<commit_message>
Changed contact details and debugged minor bugs
</commit_message>
<xml_diff>
--- a/Kategorie_Teilnehmer_Kämpfer.xlsx
+++ b/Kategorie_Teilnehmer_Kämpfer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\SV-Tora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7B865C-92C6-4C1E-9072-6EDF0913ACFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F557064-4C4C-4907-B15D-B67B97874DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42015" yWindow="3660" windowWidth="17280" windowHeight="8880" xr2:uid="{46169A17-C224-4497-8403-DF713CDC2671}"/>
   </bookViews>
@@ -291,50 +291,50 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -659,7 +659,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -677,15 +677,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="13"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
@@ -710,11 +710,11 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="6"/>
       <c r="J6" s="11"/>
     </row>
@@ -722,12 +722,12 @@
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="8" t="s">
-        <v>7</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>1</v>
@@ -739,561 +739,546 @@
         <v>4</v>
       </c>
       <c r="H8" s="10"/>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="15"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="25"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="26"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="22"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="20"/>
       <c r="J10" s="27"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="22"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="20"/>
       <c r="J11" s="27"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="22"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="27"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="22"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="20"/>
       <c r="J13" s="27"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="22"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="20"/>
       <c r="J14" s="27"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="22"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="20"/>
       <c r="J15" s="27"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="22"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="20"/>
       <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="22"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="20"/>
       <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="22"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="20"/>
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="22"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="20"/>
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="22"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="20"/>
       <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="22"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="20"/>
       <c r="J21" s="27"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="22"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="20"/>
       <c r="J22" s="27"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="22"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="20"/>
       <c r="J23" s="27"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="22"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="20"/>
       <c r="J24" s="27"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="22"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="20"/>
       <c r="J25" s="27"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="22"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="20"/>
       <c r="J26" s="27"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="22"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="20"/>
       <c r="J27" s="27"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="22"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="27"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="22"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="20"/>
       <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="22"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="20"/>
       <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="22"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="20"/>
       <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="22"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="20"/>
       <c r="J32" s="27"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="22"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="20"/>
       <c r="J33" s="27"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="22"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="20"/>
       <c r="J34" s="27"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="22"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="20"/>
       <c r="J35" s="27"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="22"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="20"/>
       <c r="J36" s="27"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="22"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="20"/>
       <c r="J37" s="27"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="22"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="20"/>
       <c r="J38" s="27"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="22"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="20"/>
       <c r="J39" s="27"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="22"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="20"/>
       <c r="J40" s="27"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="22"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="20"/>
       <c r="J41" s="27"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="22"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="20"/>
       <c r="J42" s="27"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="22"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="20"/>
       <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="22"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="20"/>
       <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="22"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="20"/>
       <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="22"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="20"/>
       <c r="J46" s="27"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="22"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="20"/>
       <c r="J47" s="27"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="22"/>
+      <c r="A48" s="12"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="20"/>
       <c r="J48" s="27"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="22"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="20"/>
       <c r="J49" s="27"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="22"/>
+      <c r="A50" s="12"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="20"/>
       <c r="J50" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
     <mergeCell ref="G48:H48"/>
     <mergeCell ref="G49:H49"/>
     <mergeCell ref="G50:H50"/>
@@ -1310,35 +1295,50 @@
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="82" orientation="portrait" r:id="rId1"/>

</xml_diff>